<commit_message>
Version 2.0. Failed Scenarios Runner is added
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="106">
   <si>
     <t>id</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>Liliia</t>
+  </si>
+  <si>
+    <t>Ozzi</t>
   </si>
 </sst>
 </file>
@@ -757,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>

</xml_diff>